<commit_message>
updating tm excel format
</commit_message>
<xml_diff>
--- a/tests/test_tm/traffic_kerman.xlsx
+++ b/tests/test_tm/traffic_kerman.xlsx
@@ -75,13 +75,13 @@
     <t xml:space="preserve">SLA_E1</t>
   </si>
   <si>
-    <t xml:space="preserve">Quantity_STM1_E</t>
+    <t xml:space="preserve">Quantity_STM1 Electrical</t>
   </si>
   <si>
     <t xml:space="preserve">SLA_STM1_E</t>
   </si>
   <si>
-    <t xml:space="preserve">Quantity_STM1_O</t>
+    <t xml:space="preserve">Quantity_STM1 Optical</t>
   </si>
   <si>
     <t xml:space="preserve">λ_STM1_O(nm)</t>
@@ -2098,11 +2098,11 @@
   </sheetPr>
   <dimension ref="A1:AO106"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="V1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AB10" activeCellId="0" sqref="AB10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J7" activeCellId="0" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.87890625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="8.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.02"/>
@@ -2175,7 +2175,7 @@
       <c r="AN1" s="8"/>
       <c r="AO1" s="8"/>
     </row>
-    <row r="2" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
         <v>10</v>
       </c>

</xml_diff>